<commit_message>
Update Decision column in HSI Review sheet Signed-off-by: Abdelrahman-Omar-Ali <a.abdelwahed20@gmail.com>
</commit_message>
<xml_diff>
--- a/Input documents/HSI_Review.xlsx
+++ b/Input documents/HSI_Review.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="46">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t xml:space="preserve">Document history has to be at the start and the page numbering should be updated to allow the user to navigate to any page from the table of contents section. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accepted </t>
   </si>
   <si>
     <t xml:space="preserve">There is no Reference table for the reference document , even HSI should have one and the reference is the customer Requirement for the product </t>
@@ -173,7 +176,7 @@
     <numFmt numFmtId="167" formatCode="[$-409]M/D/YYYY"/>
     <numFmt numFmtId="168" formatCode="@"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -203,12 +206,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -404,11 +401,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="33">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -425,10 +422,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -469,15 +462,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="3" borderId="10" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="10" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="10" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="10" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="3" borderId="10" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="10" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -489,7 +482,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -505,22 +498,10 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -541,7 +522,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -549,7 +530,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -702,10 +683,10 @@
   <dimension ref="B2:H18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J24" activeCellId="1" sqref="A8:H8 J24"/>
+      <selection pane="topLeft" activeCell="J24" activeCellId="1" sqref="G2:G7 J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="32.29"/>
   </cols>
@@ -760,13 +741,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
@@ -795,103 +776,103 @@
       <c r="H9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8" t="s">
+      <c r="D12" s="7"/>
+      <c r="E12" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="9" t="s">
+      <c r="F12" s="7"/>
+      <c r="G12" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H12" s="9"/>
+      <c r="H12" s="8"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="10" t="n">
+      <c r="B13" s="9" t="n">
         <v>0.1</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11" t="s">
+      <c r="D13" s="10"/>
+      <c r="E13" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="11"/>
+      <c r="F13" s="10"/>
       <c r="G13" s="3" t="s">
         <v>16</v>
       </c>
       <c r="H13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="10"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="10"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="10"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="10"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="12"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="33">
@@ -947,10 +928,10 @@
   <dimension ref="A1:L48"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="A8:H8"/>
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2:G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.60546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.71"/>
@@ -963,651 +944,654 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="34.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="18" t="s">
+    <row r="2" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23" t="s">
+      <c r="G2" s="22"/>
+      <c r="H2" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="23"/>
+      <c r="I2" s="22"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="20" t="s">
+      <c r="B3" s="18"/>
+      <c r="C3" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
     </row>
     <row r="4" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23" t="s">
+      <c r="G4" s="22"/>
+      <c r="H4" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="23"/>
+      <c r="I4" s="22"/>
+      <c r="K4" s="0" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23" t="s">
+      <c r="F5" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="23"/>
+      <c r="I5" s="22"/>
       <c r="K5" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="64.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6" s="26" t="s">
+      <c r="E6" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23" t="s">
+      <c r="F6" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="23"/>
+      <c r="I6" s="22"/>
     </row>
     <row r="7" customFormat="false" ht="52.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23" t="s">
+      <c r="E7" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="21"/>
+      <c r="I7" s="20"/>
     </row>
     <row r="8" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="24"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="21"/>
+      <c r="A8" s="17"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="20"/>
       <c r="K8" s="0" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="18"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="21"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="20"/>
       <c r="K9" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="18"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="21"/>
+      <c r="A10" s="17"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="20"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="19"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="21"/>
+      <c r="A11" s="18"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="20"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="19"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="21"/>
+      <c r="A12" s="18"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="20"/>
       <c r="K12" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L12" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="19"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="21"/>
+      <c r="A13" s="18"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="20"/>
       <c r="K13" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="19"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="21"/>
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="20"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="19"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="21"/>
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="20"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="19"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="21"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="20"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="28"/>
-      <c r="B17" s="29"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="33"/>
+      <c r="A17" s="24"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="29"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="28"/>
-      <c r="B18" s="29"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="33"/>
+      <c r="A18" s="24"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="29"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="28"/>
-      <c r="B19" s="29"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="33"/>
+      <c r="A19" s="24"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="29"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="28"/>
-      <c r="B20" s="29"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="33"/>
+      <c r="A20" s="24"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="29"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="28"/>
-      <c r="B21" s="29"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="33"/>
+      <c r="A21" s="24"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="29"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="28"/>
-      <c r="B22" s="29"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="35"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="23"/>
-      <c r="I22" s="33"/>
+      <c r="A22" s="24"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="29"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="28"/>
-      <c r="B23" s="29"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="33"/>
+      <c r="A23" s="24"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="29"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="28"/>
-      <c r="B24" s="29"/>
-      <c r="C24" s="30"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="35"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="33"/>
+      <c r="A24" s="24"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="29"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="28"/>
-      <c r="B25" s="29"/>
-      <c r="C25" s="30"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="23"/>
-      <c r="I25" s="33"/>
+      <c r="A25" s="24"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="29"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="28"/>
-      <c r="B26" s="29"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="33"/>
+      <c r="A26" s="24"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="29"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="28"/>
-      <c r="B27" s="29"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="23"/>
-      <c r="I27" s="33"/>
+      <c r="A27" s="24"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="29"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="28"/>
-      <c r="B28" s="29"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="33"/>
+      <c r="A28" s="24"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="29"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="30"/>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="35"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="23"/>
-      <c r="I29" s="33"/>
+      <c r="A29" s="26"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="29"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="28"/>
-      <c r="B30" s="29"/>
-      <c r="C30" s="29"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="35"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="23"/>
-      <c r="I30" s="33"/>
+      <c r="A30" s="24"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="29"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="28"/>
-      <c r="B31" s="29"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="34"/>
-      <c r="F31" s="35"/>
-      <c r="G31" s="23"/>
-      <c r="H31" s="23"/>
-      <c r="I31" s="33"/>
+      <c r="A31" s="24"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="29"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="28"/>
-      <c r="B32" s="29"/>
-      <c r="C32" s="29"/>
-      <c r="D32" s="30"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="36"/>
-      <c r="G32" s="23"/>
-      <c r="H32" s="23"/>
-      <c r="I32" s="33"/>
+      <c r="A32" s="24"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="25"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="29"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="30"/>
-      <c r="B33" s="30"/>
-      <c r="C33" s="30"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="35"/>
-      <c r="G33" s="23"/>
-      <c r="H33" s="23"/>
-      <c r="I33" s="33"/>
+      <c r="A33" s="26"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="31"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="29"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="30"/>
-      <c r="B34" s="30"/>
-      <c r="C34" s="30"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="35"/>
-      <c r="G34" s="23"/>
-      <c r="H34" s="23"/>
-      <c r="I34" s="33"/>
+      <c r="A34" s="26"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="31"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="29"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="28"/>
-      <c r="B35" s="29"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="29"/>
-      <c r="E35" s="34"/>
-      <c r="F35" s="35"/>
-      <c r="G35" s="23"/>
-      <c r="H35" s="23"/>
-      <c r="I35" s="33"/>
+      <c r="A35" s="24"/>
+      <c r="B35" s="25"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="31"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="29"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="30"/>
-      <c r="B36" s="30"/>
-      <c r="C36" s="30"/>
-      <c r="D36" s="30"/>
-      <c r="E36" s="31"/>
-      <c r="F36" s="35"/>
-      <c r="G36" s="23"/>
-      <c r="H36" s="23"/>
-      <c r="I36" s="33"/>
+      <c r="A36" s="26"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="31"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="29"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="30"/>
-      <c r="B37" s="30"/>
-      <c r="C37" s="30"/>
-      <c r="D37" s="30"/>
-      <c r="E37" s="31"/>
-      <c r="F37" s="35"/>
-      <c r="G37" s="23"/>
-      <c r="H37" s="23"/>
-      <c r="I37" s="33"/>
+      <c r="A37" s="26"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="31"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="29"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="30"/>
-      <c r="B38" s="30"/>
-      <c r="C38" s="30"/>
-      <c r="D38" s="30"/>
-      <c r="E38" s="31"/>
-      <c r="F38" s="35"/>
-      <c r="G38" s="23"/>
-      <c r="H38" s="23"/>
-      <c r="I38" s="33"/>
+      <c r="A38" s="26"/>
+      <c r="B38" s="26"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="31"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="22"/>
+      <c r="I38" s="29"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="30"/>
-      <c r="B39" s="30"/>
-      <c r="C39" s="30"/>
-      <c r="D39" s="30"/>
-      <c r="E39" s="31"/>
-      <c r="F39" s="35"/>
-      <c r="G39" s="23"/>
-      <c r="H39" s="23"/>
-      <c r="I39" s="33"/>
+      <c r="A39" s="26"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="31"/>
+      <c r="G39" s="22"/>
+      <c r="H39" s="22"/>
+      <c r="I39" s="29"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="30"/>
-      <c r="B40" s="30"/>
-      <c r="C40" s="30"/>
-      <c r="D40" s="30"/>
-      <c r="E40" s="31"/>
-      <c r="F40" s="35"/>
-      <c r="G40" s="23"/>
-      <c r="H40" s="23"/>
-      <c r="I40" s="33"/>
+      <c r="A40" s="26"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="26"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="31"/>
+      <c r="G40" s="22"/>
+      <c r="H40" s="22"/>
+      <c r="I40" s="29"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="30"/>
-      <c r="B41" s="30"/>
-      <c r="C41" s="30"/>
-      <c r="D41" s="30"/>
-      <c r="E41" s="31"/>
-      <c r="F41" s="35"/>
-      <c r="G41" s="23"/>
-      <c r="H41" s="23"/>
-      <c r="I41" s="33"/>
+      <c r="A41" s="26"/>
+      <c r="B41" s="26"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="27"/>
+      <c r="F41" s="31"/>
+      <c r="G41" s="22"/>
+      <c r="H41" s="22"/>
+      <c r="I41" s="29"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="30"/>
-      <c r="B42" s="30"/>
-      <c r="C42" s="30"/>
-      <c r="D42" s="30"/>
-      <c r="E42" s="31"/>
-      <c r="F42" s="35"/>
-      <c r="G42" s="23"/>
-      <c r="H42" s="23"/>
-      <c r="I42" s="33"/>
+      <c r="A42" s="26"/>
+      <c r="B42" s="26"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="27"/>
+      <c r="F42" s="31"/>
+      <c r="G42" s="22"/>
+      <c r="H42" s="22"/>
+      <c r="I42" s="29"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="30"/>
-      <c r="B43" s="30"/>
-      <c r="C43" s="30"/>
-      <c r="D43" s="30"/>
-      <c r="E43" s="31"/>
-      <c r="F43" s="35"/>
-      <c r="G43" s="23"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="33"/>
+      <c r="A43" s="26"/>
+      <c r="B43" s="26"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="27"/>
+      <c r="F43" s="31"/>
+      <c r="G43" s="22"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="29"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="30"/>
-      <c r="B44" s="30"/>
-      <c r="C44" s="30"/>
-      <c r="D44" s="30"/>
-      <c r="E44" s="31"/>
-      <c r="F44" s="35"/>
-      <c r="G44" s="23"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="33"/>
+      <c r="A44" s="26"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="26"/>
+      <c r="D44" s="26"/>
+      <c r="E44" s="27"/>
+      <c r="F44" s="31"/>
+      <c r="G44" s="22"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="29"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="30"/>
-      <c r="B45" s="30"/>
-      <c r="C45" s="30"/>
-      <c r="D45" s="30"/>
-      <c r="E45" s="31"/>
-      <c r="F45" s="35"/>
-      <c r="G45" s="23"/>
-      <c r="H45" s="23"/>
-      <c r="I45" s="33"/>
+      <c r="A45" s="26"/>
+      <c r="B45" s="26"/>
+      <c r="C45" s="26"/>
+      <c r="D45" s="26"/>
+      <c r="E45" s="27"/>
+      <c r="F45" s="31"/>
+      <c r="G45" s="22"/>
+      <c r="H45" s="22"/>
+      <c r="I45" s="29"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="30"/>
-      <c r="B46" s="30"/>
-      <c r="C46" s="30"/>
-      <c r="D46" s="30"/>
-      <c r="E46" s="31"/>
-      <c r="F46" s="35"/>
-      <c r="G46" s="23"/>
-      <c r="H46" s="23"/>
-      <c r="I46" s="33"/>
+      <c r="A46" s="26"/>
+      <c r="B46" s="26"/>
+      <c r="C46" s="26"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="27"/>
+      <c r="F46" s="31"/>
+      <c r="G46" s="22"/>
+      <c r="H46" s="22"/>
+      <c r="I46" s="29"/>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="30"/>
-      <c r="B47" s="30"/>
-      <c r="C47" s="30"/>
-      <c r="D47" s="30"/>
-      <c r="E47" s="31"/>
-      <c r="F47" s="35"/>
-      <c r="G47" s="23"/>
-      <c r="H47" s="23"/>
-      <c r="I47" s="33"/>
+      <c r="A47" s="26"/>
+      <c r="B47" s="26"/>
+      <c r="C47" s="26"/>
+      <c r="D47" s="26"/>
+      <c r="E47" s="27"/>
+      <c r="F47" s="31"/>
+      <c r="G47" s="22"/>
+      <c r="H47" s="22"/>
+      <c r="I47" s="29"/>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="30"/>
-      <c r="B48" s="30"/>
-      <c r="C48" s="30"/>
-      <c r="D48" s="30"/>
-      <c r="E48" s="31"/>
-      <c r="F48" s="35"/>
-      <c r="G48" s="23"/>
-      <c r="H48" s="23"/>
-      <c r="I48" s="33"/>
+      <c r="A48" s="26"/>
+      <c r="B48" s="26"/>
+      <c r="C48" s="26"/>
+      <c r="D48" s="26"/>
+      <c r="E48" s="27"/>
+      <c r="F48" s="31"/>
+      <c r="G48" s="22"/>
+      <c r="H48" s="22"/>
+      <c r="I48" s="29"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1">
@@ -1629,13 +1613,17 @@
       <formula>#ref!</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G1:G1048" type="list">
+  <dataValidations count="3">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G1 G8:G1048" type="list">
       <formula1>$K$5:$K$5</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H1:H1048" type="list">
       <formula1>$K$8:$K$9</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G2:G7" type="list">
+      <formula1>$K$4:$K$5</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>